<commit_message>
lesson 16 - rdbms - 10.11.2023
</commit_message>
<xml_diff>
--- a/JAVA 19 20 - Quyen Phan - Database Design.xlsx
+++ b/JAVA 19 20 - Quyen Phan - Database Design.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2D65D6-AD9C-40DC-93B9-D7724A34C9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3227887-AC1E-45D8-B9C0-B199E8E81E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="0" windowWidth="21600" windowHeight="12735" tabRatio="422" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="422" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
     <sheet name="B2. Mô hình logic" sheetId="2" r:id="rId2"/>
     <sheet name="B3. Mô hình quan hệ" sheetId="3" r:id="rId3"/>
     <sheet name="4. Cơ sở dữ liệu vật lý" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -71,30 +72,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Đã đặt hàng, đang đóng gói, đang giao, giao thành công, giao thất bại</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="S13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
@@ -127,6 +104,11 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
+    <author>tc={60DC5D74-2615-4FEF-BFAB-6545C6361F9E}</author>
+    <author>tc={2FA75419-8410-487C-B1BC-8CCFDA150F9B}</author>
+    <author>tc={0E88F402-66E8-4C27-90A1-9363F4A5299B}</author>
+    <author>tc={798CF2D4-2E7B-48C4-8D16-5D288974D408}</author>
+    <author>tc={38456966-9ABF-40FF-8702-70C003B001DF}</author>
   </authors>
   <commentList>
     <comment ref="W4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
@@ -153,28 +135,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="J10" authorId="1" shapeId="0" xr:uid="{60DC5D74-2615-4FEF-BFAB-6545C6361F9E}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Đã đặt hàng, đang đóng gói, đang giao, giao thành công, giao thất bại</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Amount of items still in warehouse</t>
       </text>
     </comment>
     <comment ref="W13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
@@ -201,12 +167,46 @@
         </r>
       </text>
     </comment>
+    <comment ref="B102" authorId="2" shapeId="0" xr:uid="{2FA75419-8410-487C-B1BC-8CCFDA150F9B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Là khóa ngoại liên kết đến khóa chính ID của bảng ORDER</t>
+      </text>
+    </comment>
+    <comment ref="C102" authorId="3" shapeId="0" xr:uid="{0E88F402-66E8-4C27-90A1-9363F4A5299B}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Là khóa ngoại liên kết đến khóa chính ID của bảng ITEM
+</t>
+      </text>
+    </comment>
+    <comment ref="C112" authorId="4" shapeId="0" xr:uid="{798CF2D4-2E7B-48C4-8D16-5D288974D408}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Là khóa ngoại liên kết đến khóa chính ID của bảng ORDER</t>
+      </text>
+    </comment>
+    <comment ref="D112" authorId="5" shapeId="0" xr:uid="{38456966-9ABF-40FF-8702-70C003B001DF}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Là khóa ngoại liên kết đến khóa chính ID của bảng ITEM
+</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="228">
   <si>
     <t>Xác định các đối tượng cần lưu trữ
 Xác định các thuộc tính, thông tin của từng đối tượng</t>
@@ -331,12 +331,6 @@
   </si>
   <si>
     <t>T12</t>
-  </si>
-  <si>
-    <t>1. Xác định các bảng</t>
-  </si>
-  <si>
-    <t>2. Xác định lại các thuộc tính(đơn) của từng bảng</t>
   </si>
   <si>
     <t>3. Xác định khóa chính</t>
@@ -775,6 +769,322 @@
   </si>
   <si>
     <t>15/12/2030</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>S - M - L</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>DEPARTMENT</t>
+  </si>
+  <si>
+    <t>SALES_PRICE</t>
+  </si>
+  <si>
+    <t>BUY_PRICE</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>XXL</t>
+  </si>
+  <si>
+    <t>XXXL</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>Size S Nữ</t>
+  </si>
+  <si>
+    <t>Khóa: KEY, GENDER --&gt; các cặp dữ liệu khác nhau</t>
+  </si>
+  <si>
+    <t>Khóa: ID --&gt; các id khác nhau, yêu cầu các cặp key, gender cũng phải khác nhau, thêm ràng buộc UNIQUE cho key, gender</t>
+  </si>
+  <si>
+    <t>SIZE_ID</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>TH1: Nếu 1 Item 1 Size có nhiều Color, 1 Item 1 Color có nhiều Size --&gt; Unique Item, Size, Color</t>
+  </si>
+  <si>
+    <t>TH2: 1 Item 1 Size 1 Color --&gt; Unique Item, Size</t>
+  </si>
+  <si>
+    <t>TH3: 1 Iem có 1 Color --&gt; Bỏ Color qua bảng Item</t>
+  </si>
+  <si>
+    <t>1. Xác định các bảng(table)</t>
+  </si>
+  <si>
+    <t>2. Xác định lại các thuộc tính(đơn)(column) của từng bảng</t>
+  </si>
+  <si>
+    <t>--&gt; đảm bảo các bảng dữ liệu sẽ liên kết, ràng buộc với nhau</t>
+  </si>
+  <si>
+    <t>--&gt; tránh sai sót dữ liệu</t>
+  </si>
+  <si>
+    <t>--&gt; để xử lý ràng buộc --&gt; khóa ngoại(thuộc tính dùng để liên kết 2 hay nhiều bảng với nhau)</t>
+  </si>
+  <si>
+    <t>TH3: Quan hệ n-n</t>
+  </si>
+  <si>
+    <t>TH1: Quan hệ 1-n</t>
+  </si>
+  <si>
+    <t>Item A</t>
+  </si>
+  <si>
+    <t>Item B</t>
+  </si>
+  <si>
+    <t>Item C</t>
+  </si>
+  <si>
+    <t>GROUP 1</t>
+  </si>
+  <si>
+    <t>GROUP 2</t>
+  </si>
+  <si>
+    <t>GROUP 3</t>
+  </si>
+  <si>
+    <t>Item D</t>
+  </si>
+  <si>
+    <t>Lý thuyết: Khi 2 tables có quan hệ 1-n --&gt; 'bỏ 1 vào nhiều' có nghĩa là mình sẽ tạo column khóa ngoại bên bảng n(nhiều)</t>
+  </si>
+  <si>
+    <t>Sau đó tạo liên kết ràng buộc khóa ngoại đó với khóa chính của bảng 1</t>
+  </si>
+  <si>
+    <t>ITEM_GROUP_ID</t>
+  </si>
+  <si>
+    <t>Miền giá trị của khóa ngoại trong bảng N phải giống với miền giá trị của khóa chính trong bảng 1</t>
+  </si>
+  <si>
+    <t>Bảng 1 - Cha</t>
+  </si>
+  <si>
+    <t>Bảng N - Con</t>
+  </si>
+  <si>
+    <t>TH2: Quan hệ 1-1</t>
+  </si>
+  <si>
+    <t>CREATED_BY</t>
+  </si>
+  <si>
+    <t>PAYMENT_METHOD_ID</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>O4</t>
+  </si>
+  <si>
+    <t>12.10</t>
+  </si>
+  <si>
+    <t>22.07</t>
+  </si>
+  <si>
+    <t>05.02</t>
+  </si>
+  <si>
+    <t>NV 1</t>
+  </si>
+  <si>
+    <t>NV 2</t>
+  </si>
+  <si>
+    <t>NV 3</t>
+  </si>
+  <si>
+    <t>NV 4</t>
+  </si>
+  <si>
+    <t>Bảng 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bảng 1 </t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>NV 11</t>
+  </si>
+  <si>
+    <t>NV 21</t>
+  </si>
+  <si>
+    <t>NV 31</t>
+  </si>
+  <si>
+    <t>Lưu ý: khóa ngoại phải thêm ràng buộc là unique</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <r>
+      <t>Lý thuyết: Khi 2 tables có quan hệ 1-1 --&gt; tạo khóa ngoại ở bất kỳ table nào(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tùy bài toán</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) rồi liên kết đến khóa chính của table còn lại</t>
+    </r>
+  </si>
+  <si>
+    <t>ORDER_ID</t>
+  </si>
+  <si>
+    <t>RELATION_BO</t>
+  </si>
+  <si>
+    <t>BILL_ID(unique)</t>
+  </si>
+  <si>
+    <t>ORDER_ID(unique)</t>
+  </si>
+  <si>
+    <t>Cách làm khác khi quan hệ 1-1(không khuyến khích)</t>
+  </si>
+  <si>
+    <t>Bảng N</t>
+  </si>
+  <si>
+    <t>Khách hàng X vào mua hàng gồm 3 sản phẩm, Item A, Item C, Item D --&gt; nhân viên sẽ tạo 1 đơn hàng O2</t>
+  </si>
+  <si>
+    <t>1, 2 4</t>
+  </si>
+  <si>
+    <t>ko lưu danh sách</t>
+  </si>
+  <si>
+    <t>Item 1 luôn bán cho O2</t>
+  </si>
+  <si>
+    <t>Item 3 luôn bán cho O2</t>
+  </si>
+  <si>
+    <t>Item 4 luôn bán cho O2</t>
+  </si>
+  <si>
+    <t>Lý thuyết: Khi 2 tables có quan hệ n-n --&gt; tạo ra 1 bảng mới làm bảng trung gian liên kết 2 bảng N - N</t>
+  </si>
+  <si>
+    <t>Bảng mới sẽ có ít nhất là 2 columns(chính là 2 columns khóa ngoại mình tạo ra để liên kết về khóa chính của 2 bảng N N)</t>
+  </si>
+  <si>
+    <t>Và có thể chứa thêm các column khác</t>
+  </si>
+  <si>
+    <t>Cách 1: Chọn khóa chính là tập 2 columns(khóa ngoại)</t>
+  </si>
+  <si>
+    <t>Cách 2: Tạo ra 1 column mới làm khóa chính(thêm ràng buộc unique cho 2 columns khóa ngoại)</t>
+  </si>
+  <si>
+    <t>ORDER_DETAIL</t>
+  </si>
+  <si>
+    <t>CONSTRAINT - UNIQUE</t>
+  </si>
+  <si>
+    <t>Mô hình quan niệm</t>
+  </si>
+  <si>
+    <t>Mô hình logic</t>
+  </si>
+  <si>
+    <t>Mô hình quan hệ(cơ sở dữ liệu)</t>
+  </si>
+  <si>
+    <t>thuộc tính</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>đối tượng</t>
+  </si>
+  <si>
+    <t>thực thể</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>khóa</t>
+  </si>
+  <si>
+    <t>khóa chính</t>
+  </si>
+  <si>
+    <t>mối quan hệ</t>
+  </si>
+  <si>
+    <t>ràng buộc, khóa ngoại</t>
   </si>
 </sst>
 </file>
@@ -831,14 +1141,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -858,8 +1160,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -896,6 +1206,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -924,7 +1240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -965,23 +1281,44 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1002,7 +1339,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1020,6 +1402,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1292,12 +1678,34 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="J10" dT="2023-11-10T14:20:56.11" personId="{00000000-0000-0000-0000-000000000000}" id="{60DC5D74-2615-4FEF-BFAB-6545C6361F9E}">
+    <text>Amount of items still in warehouse</text>
+  </threadedComment>
+  <threadedComment ref="B102" dT="2023-11-10T14:13:44.93" personId="{00000000-0000-0000-0000-000000000000}" id="{2FA75419-8410-487C-B1BC-8CCFDA150F9B}">
+    <text>Là khóa ngoại liên kết đến khóa chính ID của bảng ORDER</text>
+  </threadedComment>
+  <threadedComment ref="C102" dT="2023-11-10T14:14:05.05" personId="{00000000-0000-0000-0000-000000000000}" id="{0E88F402-66E8-4C27-90A1-9363F4A5299B}">
+    <text xml:space="preserve">Là khóa ngoại liên kết đến khóa chính ID của bảng ITEM
+</text>
+  </threadedComment>
+  <threadedComment ref="C112" dT="2023-11-10T14:13:44.93" personId="{00000000-0000-0000-0000-000000000000}" id="{798CF2D4-2E7B-48C4-8D16-5D288974D408}">
+    <text>Là khóa ngoại liên kết đến khóa chính ID của bảng ORDER</text>
+  </threadedComment>
+  <threadedComment ref="D112" dT="2023-11-10T14:14:05.05" personId="{00000000-0000-0000-0000-000000000000}" id="{38456966-9ABF-40FF-8702-70C003B001DF}">
+    <text xml:space="preserve">Là khóa ngoại liên kết đến khóa chính ID của bảng ITEM
+</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:F15"/>
+    <sheetView topLeftCell="E6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" activeCellId="1" sqref="E21 E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -1318,21 +1726,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="G2" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="G2" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
     </row>
     <row r="3" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1340,7 +1748,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K3" s="1">
         <v>5</v>
@@ -1350,9 +1758,9 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1360,7 +1768,7 @@
         <v>3</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K4" s="1">
         <v>10</v>
@@ -1372,170 +1780,170 @@
     <row r="5" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>94</v>
+        <v>75</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>92</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>110</v>
+        <v>98</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>108</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>102</v>
+        <v>76</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>114</v>
+        <v>109</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>112</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>95</v>
+      <c r="B11" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>93</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>115</v>
+      <c r="G11" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>113</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -1546,7 +1954,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1561,7 +1969,7 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1576,7 +1984,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1591,7 +1999,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1605,7 +2013,7 @@
     <row r="16" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="20" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="3"/>
@@ -1661,16 +2069,16 @@
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="21" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1680,13 +2088,13 @@
       </c>
       <c r="C23" s="5"/>
       <c r="I23" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="K23" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="K23" s="20" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1697,7 +2105,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>24</v>
@@ -1711,10 +2119,10 @@
         <v>2</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1722,10 +2130,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1733,10 +2141,10 @@
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1776,10 +2184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="H3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -1787,11 +2195,12 @@
     <col min="1" max="1" width="32.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38" style="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.5703125" style="1" customWidth="1"/>
-    <col min="8" max="11" width="22.7109375" style="1" customWidth="1"/>
+    <col min="8" max="10" width="22.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.85546875" style="1" customWidth="1"/>
     <col min="12" max="12" width="30.5703125" style="1" customWidth="1"/>
     <col min="13" max="101" width="22.7109375" style="1" customWidth="1"/>
     <col min="102" max="16384" width="9.140625" style="1"/>
@@ -1799,16 +2208,16 @@
   <sheetData>
     <row r="1" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
     </row>
     <row r="3" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1817,9 +2226,9 @@
       </c>
     </row>
     <row r="4" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1884,70 +2293,165 @@
       <c r="S5" s="11"/>
     </row>
     <row r="6" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="B7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="M8" s="3"/>
       <c r="Q8" s="9"/>
     </row>
     <row r="9" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>142</v>
+      </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="30" t="s">
+        <v>79</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>133</v>
+      </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1955,13 +2459,21 @@
       <c r="R10" s="10"/>
     </row>
     <row r="11" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -1969,12 +2481,18 @@
       <c r="M11" s="3"/>
     </row>
     <row r="12" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="L12" s="3"/>
@@ -1982,8 +2500,12 @@
     </row>
     <row r="13" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>13</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1998,7 +2520,9 @@
     <row r="14" spans="2:19" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="25" t="s">
+        <v>99</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -2036,6 +2560,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -2086,9 +2611,13 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F20" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="21" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="35" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -2097,14 +2626,22 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="F21" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="G21" s="6"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
+      <c r="H21" s="13">
+        <v>1</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="J21" s="27">
+        <v>44119</v>
+      </c>
     </row>
     <row r="22" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="28"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
@@ -2131,8 +2668,8 @@
       <c r="J23" s="13"/>
     </row>
     <row r="24" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="29" t="s">
-        <v>71</v>
+      <c r="A24" s="36" t="s">
+        <v>69</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>18</v>
@@ -2147,7 +2684,7 @@
       <c r="J24" s="13"/>
     </row>
     <row r="25" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="30"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="7" t="s">
         <v>19</v>
       </c>
@@ -2176,27 +2713,27 @@
     <row r="29" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2207,100 +2744,382 @@
         <v>24</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F32" s="31">
+        <v>123</v>
+      </c>
+      <c r="F32" s="24">
         <v>44114</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F34" s="31">
+        <v>125</v>
+      </c>
+      <c r="F34" s="24">
         <v>35715</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G36" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="I38" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J39" s="1">
+        <v>15</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>2</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E40" s="31">
+        <v>120</v>
+      </c>
+      <c r="E40" s="24">
         <v>35715</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="G40" s="1">
+        <v>2</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J40" s="1">
+        <v>20</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G41" s="1">
+        <v>3</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J41" s="1">
+        <v>22</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H42" s="1">
+        <v>2</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>6</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
+        <v>7</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G50" s="1">
+        <v>1</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
+        <v>8</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1">
+        <v>2</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I51" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
+        <v>9</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="G52" s="1">
+        <v>3</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I52" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
+        <v>10</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>11</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>12</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:D4"/>
@@ -2315,21 +3134,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:W51"/>
+  <dimension ref="A1:W118"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:G1"/>
+    <sheetView topLeftCell="A92" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
     <col min="2" max="3" width="30.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="36.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" style="1" customWidth="1"/>
     <col min="9" max="9" width="53.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="22.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="28.5703125" style="1" customWidth="1"/>
@@ -2341,18 +3160,18 @@
   <sheetData>
     <row r="1" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="1" t="s">
@@ -2363,9 +3182,9 @@
       </c>
     </row>
     <row r="4" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="1" t="s">
@@ -2394,53 +3213,53 @@
       </c>
     </row>
     <row r="5" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="18" t="s">
         <v>35</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="M5" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="N5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="Q5" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="P5" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" s="19" t="s">
-        <v>51</v>
       </c>
       <c r="S5" s="1">
         <v>1</v>
@@ -2459,137 +3278,226 @@
       </c>
     </row>
     <row r="6" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="B7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="U8" s="9"/>
     </row>
     <row r="9" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="B9" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>142</v>
+      </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="J9" s="30" t="s">
+        <v>79</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>133</v>
+      </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="U10" s="9"/>
       <c r="V10" s="10"/>
     </row>
     <row r="11" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="25" t="s">
+        <v>13</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -2599,16 +3507,15 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="U13" s="12"/>
     </row>
     <row r="14" spans="2:23" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="25" t="s">
+        <v>99</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -2618,9 +3525,6 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
       <c r="U14" s="9"/>
       <c r="V14" s="10"/>
@@ -2638,9 +3542,6 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
       <c r="U15" s="9"/>
       <c r="V15" s="10"/>
@@ -2658,8 +3559,6 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="U16" s="9"/>
       <c r="V16" s="10"/>
@@ -2677,9 +3576,6 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="U17" s="9"/>
       <c r="V17" s="10"/>
@@ -2697,9 +3593,6 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2715,19 +3608,16 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
-      <c r="B21" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
+      <c r="B21" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -2735,7 +3625,7 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
@@ -2743,11 +3633,11 @@
     </row>
     <row r="22" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="14"/>
-      <c r="B22" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="B22" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -2755,18 +3645,18 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
       <c r="N22" s="13"/>
     </row>
     <row r="23" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
+      <c r="B23" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -2774,18 +3664,18 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
     </row>
     <row r="24" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
+      <c r="B24" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
@@ -2798,7 +3688,9 @@
       <c r="N24" s="13"/>
     </row>
     <row r="25" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="6"/>
+      <c r="B25" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -2811,36 +3703,837 @@
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="38" t="s">
+        <v>155</v>
+      </c>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="38" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="28" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="3">
+        <v>100</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <v>2</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="3">
+        <v>200</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <v>3</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" s="3">
+        <v>300</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>4</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="3">
+        <v>400</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="3">
+        <v>2</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="3">
+        <v>3</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C58" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E59" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C60" s="3">
+        <v>18.09</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E60" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C61" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D65" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="F65" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="G65" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="H65" s="44"/>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D66" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D67" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D68" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="F68" s="3">
+        <v>2</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D69" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="F69" s="3">
+        <v>3</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F70" s="3">
+        <v>4</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="4"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C84" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="E84" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="F84" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="G84" s="47"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E85" s="3">
+        <v>1</v>
+      </c>
+      <c r="F85" s="47"/>
+      <c r="G85" s="47"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E86" s="3">
+        <v>2</v>
+      </c>
+      <c r="F86" s="47" t="s">
+        <v>204</v>
+      </c>
+      <c r="G86" s="47" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C87" s="3">
+        <v>18.09</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E87" s="3">
+        <v>2</v>
+      </c>
+      <c r="F87" s="47"/>
+      <c r="G87" s="47"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C88" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E88" s="3">
+        <v>1</v>
+      </c>
+      <c r="F88" s="47"/>
+      <c r="G88" s="47"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F89" s="47"/>
+      <c r="G89" s="47"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F90" s="47"/>
+      <c r="G90" s="47"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="F91" s="47"/>
+      <c r="G91" s="47"/>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B92" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C92" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D92" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E92" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="F92" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="G92" s="47"/>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="3">
+        <v>1</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D93" s="3">
+        <v>100</v>
+      </c>
+      <c r="E93" s="3">
+        <v>1</v>
+      </c>
+      <c r="F93" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="G93" s="47" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B94" s="3">
+        <v>2</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D94" s="3">
+        <v>200</v>
+      </c>
+      <c r="E94" s="3">
+        <v>1</v>
+      </c>
+      <c r="F94" s="47"/>
+      <c r="G94" s="47"/>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B95" s="3">
+        <v>3</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D95" s="3">
+        <v>300</v>
+      </c>
+      <c r="E95" s="3">
+        <v>2</v>
+      </c>
+      <c r="F95" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="G95" s="47" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B96" s="3">
+        <v>4</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D96" s="3">
+        <v>400</v>
+      </c>
+      <c r="E96" s="3">
+        <v>1</v>
+      </c>
+      <c r="F96" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="G96" s="47" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="46" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="C102" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C103" s="3">
+        <v>1</v>
+      </c>
+      <c r="D103" s="3">
+        <v>10</v>
+      </c>
+      <c r="E103" s="12"/>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B104" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C104" s="3">
+        <v>2</v>
+      </c>
+      <c r="D104" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C105" s="3">
+        <v>4</v>
+      </c>
+      <c r="D105" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B106" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C106" s="3">
+        <v>5</v>
+      </c>
+      <c r="D106" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C107" s="3">
+        <v>6</v>
+      </c>
+      <c r="D107" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B108" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C108" s="3">
+        <v>6</v>
+      </c>
+      <c r="D108" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="C111" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="D111" s="50"/>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B112" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C112" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="D112" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113" s="3">
+        <v>1</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D113" s="3">
+        <v>1</v>
+      </c>
+      <c r="E113" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" s="3">
+        <v>2</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D114" s="3">
+        <v>2</v>
+      </c>
+      <c r="E114" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B115" s="3">
+        <v>3</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D115" s="3">
+        <v>4</v>
+      </c>
+      <c r="E115" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="3">
+        <v>4</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D116" s="3">
+        <v>5</v>
+      </c>
+      <c r="E116" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="3">
+        <v>5</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D117" s="3">
+        <v>6</v>
+      </c>
+      <c r="E117" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="3">
+        <v>6</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D118" s="3">
+        <v>6</v>
+      </c>
+      <c r="E118" s="3">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:D4"/>
+    <mergeCell ref="C111:D111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2852,8 +4545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A45"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.25"/>
@@ -2864,99 +4557,99 @@
   <sheetData>
     <row r="1" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2987,4 +4680,88 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D63DB90-5A83-43F6-9FC7-66B118A6C626}">
+  <dimension ref="B2:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="13" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="53" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="53" t="s">
+        <v>221</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="53"/>
+      <c r="C5" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="53" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="53"/>
+      <c r="C6" s="52" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="53"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="53" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C6:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>